<commit_message>
Started work on the next Carrier Board
</commit_message>
<xml_diff>
--- a/Documents/TMC-Carrier-Board 3.02.2025 .xlsx
+++ b/Documents/TMC-Carrier-Board 3.02.2025 .xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vovmo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vovmo\Documents\Bäumlihof 3A\Maturaarbeit\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A3631D1-2EA2-4E3B-9AEC-748B279ADEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B451C758-3A9A-4909-AC94-A40E07A8DD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DB1B8C9D-9720-45D7-8FC6-60548039E79F}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{DB1B8C9D-9720-45D7-8FC6-60548039E79F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +541,7 @@
         <v>0.09</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="0">B3*D3</f>
+        <f t="shared" ref="E3:E7" si="0">B3*D3</f>
         <v>0.63</v>
       </c>
     </row>

</xml_diff>